<commit_message>
data processor added and appendix code changed to NOT redundant
</commit_message>
<xml_diff>
--- a/Implementation/Python/model2/M2_output_alloc.xlsx
+++ b/Implementation/Python/model2/M2_output_alloc.xlsx
@@ -5335,7 +5335,7 @@
         <v>1</v>
       </c>
       <c r="AB10">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AC10">
         <v>0</v>
@@ -5889,19 +5889,19 @@
         <v>0</v>
       </c>
       <c r="AE11">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AF11">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AG11">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AH11">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AI11">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AJ11">
         <v>0</v>
@@ -6419,13 +6419,13 @@
         <v>0</v>
       </c>
       <c r="Z12">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AA12">
         <v>0</v>
       </c>
       <c r="AB12">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AC12">
         <v>0</v>
@@ -6452,10 +6452,10 @@
         <v>1</v>
       </c>
       <c r="AK12">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AL12">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AM12">
         <v>0</v>
@@ -6949,13 +6949,13 @@
         <v>0</v>
       </c>
       <c r="U13">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="V13">
         <v>0</v>
       </c>
       <c r="W13">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="X13">
         <v>0</v>
@@ -7006,19 +7006,19 @@
         <v>1</v>
       </c>
       <c r="AN13">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AO13">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AP13">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AQ13">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AR13">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AS13">
         <v>0</v>
@@ -7509,7 +7509,7 @@
         <v>0</v>
       </c>
       <c r="Z14">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AA14">
         <v>0</v>
@@ -7518,7 +7518,7 @@
         <v>0</v>
       </c>
       <c r="AC14">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AD14">
         <v>0</v>
@@ -7527,7 +7527,7 @@
         <v>0</v>
       </c>
       <c r="AF14">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AG14">
         <v>0</v>
@@ -7563,25 +7563,25 @@
         <v>0</v>
       </c>
       <c r="AR14">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AS14">
         <v>1</v>
       </c>
       <c r="AT14">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AU14">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AV14">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AW14">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AX14">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AY14">
         <v>0</v>
@@ -8650,10 +8650,10 @@
         <v>0</v>
       </c>
       <c r="AQ16">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AR16">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AS16">
         <v>0</v>
@@ -8695,10 +8695,10 @@
         <v>1</v>
       </c>
       <c r="BF16">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="BG16">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="BH16">
         <v>0</v>
@@ -9713,7 +9713,7 @@
         <v>0</v>
       </c>
       <c r="AH18">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AI18">
         <v>0</v>
@@ -9752,7 +9752,7 @@
         <v>0</v>
       </c>
       <c r="AU18">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AV18">
         <v>0</v>
@@ -9800,7 +9800,7 @@
         <v>0</v>
       </c>
       <c r="BK18">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="BL18">
         <v>0</v>
@@ -10234,14 +10234,14 @@
         <v>0</v>
       </c>
       <c r="Z19">
+        <v>-0</v>
+      </c>
+      <c r="AA19">
+        <v>0</v>
+      </c>
+      <c r="AB19">
         <v>1</v>
       </c>
-      <c r="AA19">
-        <v>0</v>
-      </c>
-      <c r="AB19">
-        <v>0</v>
-      </c>
       <c r="AC19">
         <v>0</v>
       </c>
@@ -10258,7 +10258,7 @@
         <v>0</v>
       </c>
       <c r="AH19">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AI19">
         <v>0</v>
@@ -11336,7 +11336,7 @@
         <v>0</v>
       </c>
       <c r="AD21">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AE21">
         <v>0</v>
@@ -12016,7 +12016,7 @@
         <v>0</v>
       </c>
       <c r="BW22">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="BX22">
         <v>1</v>
@@ -12414,7 +12414,7 @@
         <v>0</v>
       </c>
       <c r="Z23">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AA23">
         <v>0</v>
@@ -12459,7 +12459,7 @@
         <v>0</v>
       </c>
       <c r="AO23">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AP23">
         <v>0</v>
@@ -12522,7 +12522,7 @@
         <v>0</v>
       </c>
       <c r="BJ23">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="BK23">
         <v>0</v>
@@ -12983,7 +12983,7 @@
         <v>0</v>
       </c>
       <c r="AH24">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AI24">
         <v>0</v>
@@ -13118,13 +13118,13 @@
         <v>0</v>
       </c>
       <c r="CA24">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="CB24">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="CC24">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="CD24">
         <v>0</v>
@@ -13549,7 +13549,7 @@
         <v>0</v>
       </c>
       <c r="AO25">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AP25">
         <v>0</v>
@@ -13675,7 +13675,7 @@
         <v>0</v>
       </c>
       <c r="CE25">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="CF25">
         <v>0</v>
@@ -14070,7 +14070,7 @@
         <v>0</v>
       </c>
       <c r="AG26">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AH26">
         <v>1</v>
@@ -14094,7 +14094,7 @@
         <v>0</v>
       </c>
       <c r="AO26">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AP26">
         <v>0</v>
@@ -14103,7 +14103,7 @@
         <v>0</v>
       </c>
       <c r="AR26">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AS26">
         <v>0</v>
@@ -14594,13 +14594,13 @@
         <v>0</v>
       </c>
       <c r="Z27">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AA27">
         <v>0</v>
       </c>
       <c r="AB27">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AC27">
         <v>1</v>
@@ -14768,7 +14768,7 @@
         <v>0</v>
       </c>
       <c r="CF27">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="CG27">
         <v>0</v>
@@ -15157,10 +15157,10 @@
         <v>0</v>
       </c>
       <c r="AF28">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AG28">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AH28">
         <v>0</v>
@@ -15208,7 +15208,7 @@
         <v>0</v>
       </c>
       <c r="AW28">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AX28">
         <v>0</v>
@@ -15247,10 +15247,10 @@
         <v>0</v>
       </c>
       <c r="BJ28">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="BK28">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="BL28">
         <v>0</v>
@@ -15295,7 +15295,7 @@
         <v>0</v>
       </c>
       <c r="BZ28">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="CA28">
         <v>0</v>
@@ -15319,7 +15319,7 @@
         <v>1</v>
       </c>
       <c r="CH28">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="CI28">
         <v>0</v>
@@ -16247,7 +16247,7 @@
         <v>0</v>
       </c>
       <c r="AF30">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AG30">
         <v>0</v>
@@ -16340,7 +16340,7 @@
         <v>0</v>
       </c>
       <c r="BK30">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="BL30">
         <v>0</v>
@@ -16406,7 +16406,7 @@
         <v>0</v>
       </c>
       <c r="CG30">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="CH30">
         <v>0</v>
@@ -16801,7 +16801,7 @@
         <v>0</v>
       </c>
       <c r="AI31">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AJ31">
         <v>0</v>
@@ -16975,10 +16975,10 @@
         <v>1</v>
       </c>
       <c r="CO31">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="CP31">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="CQ31">
         <v>0</v>
@@ -18412,7 +18412,7 @@
         <v>0</v>
       </c>
       <c r="AA34">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AB34">
         <v>0</v>
@@ -18421,7 +18421,7 @@
         <v>0</v>
       </c>
       <c r="AD34">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AE34">
         <v>0</v>
@@ -18460,10 +18460,10 @@
         <v>0</v>
       </c>
       <c r="AQ34">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AR34">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AS34">
         <v>0</v>
@@ -19490,7 +19490,7 @@
         <v>0</v>
       </c>
       <c r="W36">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="X36">
         <v>0</v>
@@ -19499,13 +19499,13 @@
         <v>0</v>
       </c>
       <c r="Z36">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AA36">
         <v>0</v>
       </c>
       <c r="AB36">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AC36">
         <v>0</v>
@@ -19550,7 +19550,7 @@
         <v>0</v>
       </c>
       <c r="AQ36">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AR36">
         <v>0</v>
@@ -19559,7 +19559,7 @@
         <v>0</v>
       </c>
       <c r="AT36">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AU36">
         <v>0</v>
@@ -21134,13 +21134,13 @@
         <v>0</v>
       </c>
       <c r="Z39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA39">
         <v>0</v>
       </c>
       <c r="AB39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC39">
         <v>0</v>
@@ -21158,7 +21158,7 @@
         <v>0</v>
       </c>
       <c r="AH39">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AI39">
         <v>0</v>
@@ -21179,13 +21179,13 @@
         <v>0</v>
       </c>
       <c r="AO39">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AP39">
         <v>0</v>
       </c>
       <c r="AQ39">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AR39">
         <v>0</v>
@@ -21685,7 +21685,7 @@
         <v>0</v>
       </c>
       <c r="AB40">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AC40">
         <v>0</v>
@@ -21703,7 +21703,7 @@
         <v>0</v>
       </c>
       <c r="AH40">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AI40">
         <v>0</v>
@@ -21742,7 +21742,7 @@
         <v>0</v>
       </c>
       <c r="AU40">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AV40">
         <v>0</v>
@@ -21790,7 +21790,7 @@
         <v>0</v>
       </c>
       <c r="BK40">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="BL40">
         <v>0</v>
@@ -21799,7 +21799,7 @@
         <v>0</v>
       </c>
       <c r="BN40">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="BO40">
         <v>0</v>
@@ -21931,7 +21931,7 @@
         <v>1</v>
       </c>
       <c r="DF40">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="DG40">
         <v>0</v>
@@ -22224,7 +22224,7 @@
         <v>0</v>
       </c>
       <c r="Z41">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AA41">
         <v>0</v>
@@ -22248,7 +22248,7 @@
         <v>0</v>
       </c>
       <c r="AH41">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AI41">
         <v>0</v>
@@ -22335,7 +22335,7 @@
         <v>0</v>
       </c>
       <c r="BK41">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="BL41">
         <v>0</v>
@@ -22473,7 +22473,7 @@
         <v>0</v>
       </c>
       <c r="DE41">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="DF41">
         <v>0</v>
@@ -23305,7 +23305,7 @@
         <v>0</v>
       </c>
       <c r="W43">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="X43">
         <v>0</v>
@@ -23314,13 +23314,13 @@
         <v>0</v>
       </c>
       <c r="Z43">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AA43">
         <v>0</v>
       </c>
       <c r="AB43">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AC43">
         <v>0</v>
@@ -23338,7 +23338,7 @@
         <v>0</v>
       </c>
       <c r="AH43">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AI43">
         <v>0</v>
@@ -23359,7 +23359,7 @@
         <v>0</v>
       </c>
       <c r="AO43">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AP43">
         <v>0</v>
@@ -23877,7 +23877,7 @@
         <v>0</v>
       </c>
       <c r="AF44">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AG44">
         <v>0</v>
@@ -23967,7 +23967,7 @@
         <v>0</v>
       </c>
       <c r="BJ44">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="BK44">
         <v>0</v>
@@ -24015,7 +24015,7 @@
         <v>0</v>
       </c>
       <c r="BZ44">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="CA44">
         <v>0</v>
@@ -24093,7 +24093,7 @@
         <v>0</v>
       </c>
       <c r="CZ44">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="DA44">
         <v>0</v>
@@ -24398,7 +24398,7 @@
         <v>0</v>
       </c>
       <c r="X45">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="Y45">
         <v>0</v>
@@ -24419,7 +24419,7 @@
         <v>0</v>
       </c>
       <c r="AE45">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AF45">
         <v>0</v>
@@ -24587,7 +24587,7 @@
         <v>0</v>
       </c>
       <c r="CI45">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="CJ45">
         <v>0</v>
@@ -24668,7 +24668,7 @@
         <v>0</v>
       </c>
       <c r="DJ45">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="DK45">
         <v>0</v>
@@ -25216,7 +25216,7 @@
         <v>0</v>
       </c>
       <c r="DK46">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="DL46">
         <v>0</v>
@@ -25488,7 +25488,7 @@
         <v>0</v>
       </c>
       <c r="X47">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="Y47">
         <v>0</v>
@@ -25692,10 +25692,10 @@
         <v>0</v>
       </c>
       <c r="CN47">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="CO47">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="CP47">
         <v>1</v>
@@ -25767,10 +25767,10 @@
         <v>0</v>
       </c>
       <c r="DM47">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="DN47">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="DO47">
         <v>0</v>
@@ -26084,7 +26084,7 @@
         <v>0</v>
       </c>
       <c r="AO48">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AP48">
         <v>0</v>
@@ -26159,7 +26159,7 @@
         <v>0</v>
       </c>
       <c r="BN48">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="BO48">
         <v>0</v>
@@ -26222,7 +26222,7 @@
         <v>0</v>
       </c>
       <c r="CI48">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="CJ48">
         <v>0</v>
@@ -26318,7 +26318,7 @@
         <v>0</v>
       </c>
       <c r="DO48">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="DP48">
         <v>0</v>
@@ -26584,13 +26584,13 @@
         <v>0</v>
       </c>
       <c r="Z49">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AA49">
         <v>0</v>
       </c>
       <c r="AB49">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AC49">
         <v>0</v>
@@ -26608,7 +26608,7 @@
         <v>0</v>
       </c>
       <c r="AH49">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AI49">
         <v>0</v>
@@ -26866,7 +26866,7 @@
         <v>0</v>
       </c>
       <c r="DP49">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="DQ49">
         <v>0</v>
@@ -27773,7 +27773,7 @@
         <v>0</v>
       </c>
       <c r="BG51">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="BH51">
         <v>0</v>
@@ -28396,7 +28396,7 @@
         <v>0</v>
       </c>
       <c r="CG52">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="CH52">
         <v>0</v>
@@ -28522,10 +28522,10 @@
         <v>1</v>
       </c>
       <c r="DW52">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="DX52">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="DY52">
         <v>0</v>
@@ -28779,10 +28779,10 @@
         <v>0</v>
       </c>
       <c r="AE53">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AF53">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AG53">
         <v>0</v>
@@ -29031,7 +29031,7 @@
         <v>0</v>
       </c>
       <c r="DK53">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="DL53">
         <v>0</v>
@@ -29309,7 +29309,7 @@
         <v>0</v>
       </c>
       <c r="Z54">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AA54">
         <v>0</v>
@@ -29962,7 +29962,7 @@
         <v>0</v>
       </c>
       <c r="BJ55">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="BK55">
         <v>0</v>
@@ -30010,7 +30010,7 @@
         <v>0</v>
       </c>
       <c r="BZ55">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="CA55">
         <v>0</v>
@@ -30402,7 +30402,7 @@
         <v>0</v>
       </c>
       <c r="AA56">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AB56">
         <v>0</v>
@@ -30414,7 +30414,7 @@
         <v>0</v>
       </c>
       <c r="AE56">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AF56">
         <v>0</v>
@@ -30962,7 +30962,7 @@
         <v>0</v>
       </c>
       <c r="AF57">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AG57">
         <v>0</v>
@@ -30992,13 +30992,13 @@
         <v>0</v>
       </c>
       <c r="AP57">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AQ57">
         <v>0</v>
       </c>
       <c r="AR57">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AS57">
         <v>0</v>
@@ -31064,7 +31064,7 @@
         <v>0</v>
       </c>
       <c r="BN57">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="BO57">
         <v>0</v>
@@ -31226,7 +31226,7 @@
         <v>0</v>
       </c>
       <c r="DP57">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="DQ57">
         <v>0</v>
@@ -31495,10 +31495,10 @@
         <v>0</v>
       </c>
       <c r="AB58">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AC58">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AD58">
         <v>0</v>
@@ -31513,7 +31513,7 @@
         <v>0</v>
       </c>
       <c r="AH58">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AI58">
         <v>0</v>
@@ -31549,10 +31549,10 @@
         <v>0</v>
       </c>
       <c r="AT58">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AU58">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AV58">
         <v>0</v>
@@ -31603,7 +31603,7 @@
         <v>0</v>
       </c>
       <c r="BL58">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="BM58">
         <v>0</v>
@@ -31657,7 +31657,7 @@
         <v>0</v>
       </c>
       <c r="CD58">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="CE58">
         <v>0</v>
@@ -33124,7 +33124,7 @@
         <v>0</v>
       </c>
       <c r="Z61">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AA61">
         <v>0</v>
@@ -33169,7 +33169,7 @@
         <v>0</v>
       </c>
       <c r="AO61">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AP61">
         <v>0</v>
@@ -33286,13 +33286,13 @@
         <v>0</v>
       </c>
       <c r="CB61">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="CC61">
         <v>0</v>
       </c>
       <c r="CD61">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="CE61">
         <v>0</v>
@@ -33487,7 +33487,7 @@
         <v>0</v>
       </c>
       <c r="EQ61">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="ER61">
         <v>0</v>
@@ -34214,13 +34214,13 @@
         <v>0</v>
       </c>
       <c r="Z63">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AA63">
         <v>0</v>
       </c>
       <c r="AB63">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AC63">
         <v>0</v>
@@ -34250,7 +34250,7 @@
         <v>0</v>
       </c>
       <c r="AL63">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AM63">
         <v>0</v>
@@ -34274,7 +34274,7 @@
         <v>0</v>
       </c>
       <c r="AT63">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AU63">
         <v>0</v>
@@ -35840,7 +35840,7 @@
         <v>0</v>
       </c>
       <c r="W66">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="X66">
         <v>0</v>
@@ -35849,7 +35849,7 @@
         <v>0</v>
       </c>
       <c r="Z66">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AA66">
         <v>0</v>
@@ -35870,7 +35870,7 @@
         <v>0</v>
       </c>
       <c r="AG66">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AH66">
         <v>0</v>
@@ -36029,7 +36029,7 @@
         <v>0</v>
       </c>
       <c r="CH66">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="CI66">
         <v>0</v>
@@ -36394,13 +36394,13 @@
         <v>0</v>
       </c>
       <c r="Z67">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AA67">
         <v>0</v>
       </c>
       <c r="AB67">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AC67">
         <v>0</v>
@@ -36418,7 +36418,7 @@
         <v>0</v>
       </c>
       <c r="AH67">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AI67">
         <v>0</v>
@@ -37493,7 +37493,7 @@
         <v>0</v>
       </c>
       <c r="AC69">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AD69">
         <v>0</v>
@@ -38032,7 +38032,7 @@
         <v>0</v>
       </c>
       <c r="AA70">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AB70">
         <v>0</v>
@@ -38044,7 +38044,7 @@
         <v>0</v>
       </c>
       <c r="AE70">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AF70">
         <v>0</v>
@@ -38365,7 +38365,7 @@
         <v>0</v>
       </c>
       <c r="EH70">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="EI70">
         <v>0</v>
@@ -39119,7 +39119,7 @@
         <v>0</v>
       </c>
       <c r="Z72">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AA72">
         <v>0</v>
@@ -39149,7 +39149,7 @@
         <v>0</v>
       </c>
       <c r="AJ72">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AK72">
         <v>0</v>
@@ -39284,7 +39284,7 @@
         <v>0</v>
       </c>
       <c r="CC72">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="CD72">
         <v>0</v>
@@ -39515,7 +39515,7 @@
         <v>0</v>
       </c>
       <c r="FB72">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="FC72">
         <v>0</v>
@@ -39673,7 +39673,7 @@
         <v>0</v>
       </c>
       <c r="AC73">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AD73">
         <v>0</v>
@@ -39733,7 +39733,7 @@
         <v>0</v>
       </c>
       <c r="AW73">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AX73">
         <v>0</v>
@@ -40209,16 +40209,16 @@
         <v>0</v>
       </c>
       <c r="Z74">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AA74">
         <v>0</v>
       </c>
       <c r="AB74">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AC74">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AD74">
         <v>0</v>
@@ -40757,7 +40757,7 @@
         <v>0</v>
       </c>
       <c r="AA75">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AB75">
         <v>0</v>
@@ -40769,10 +40769,10 @@
         <v>0</v>
       </c>
       <c r="AE75">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AF75">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AG75">
         <v>0</v>
@@ -41383,7 +41383,7 @@
         <v>0</v>
       </c>
       <c r="BB76">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="BC76">
         <v>0</v>
@@ -41452,7 +41452,7 @@
         <v>0</v>
       </c>
       <c r="BY76">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="BZ76">
         <v>0</v>
@@ -41566,7 +41566,7 @@
         <v>0</v>
       </c>
       <c r="DK76">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="DL76">
         <v>0</v>
@@ -41590,7 +41590,7 @@
         <v>0</v>
       </c>
       <c r="DS76">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="DT76">
         <v>0</v>
@@ -41599,7 +41599,7 @@
         <v>0</v>
       </c>
       <c r="DV76">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="DW76">
         <v>1</v>
@@ -41865,10 +41865,10 @@
         <v>0</v>
       </c>
       <c r="AG77">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AH77">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AI77">
         <v>0</v>
@@ -41907,7 +41907,7 @@
         <v>0</v>
       </c>
       <c r="AU77">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AV77">
         <v>0</v>
@@ -42380,7 +42380,7 @@
         <v>0</v>
       </c>
       <c r="W78">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="X78">
         <v>0</v>
@@ -42434,7 +42434,7 @@
         <v>0</v>
       </c>
       <c r="AO78">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AP78">
         <v>0</v>
@@ -42551,7 +42551,7 @@
         <v>0</v>
       </c>
       <c r="CB78">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="CC78">
         <v>0</v>
@@ -42985,7 +42985,7 @@
         <v>0</v>
       </c>
       <c r="AQ79">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AR79">
         <v>1</v>
@@ -43054,7 +43054,7 @@
         <v>0</v>
       </c>
       <c r="BN79">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="BO79">
         <v>0</v>
@@ -43096,7 +43096,7 @@
         <v>0</v>
       </c>
       <c r="CB79">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="CC79">
         <v>0</v>
@@ -43485,7 +43485,7 @@
         <v>0</v>
       </c>
       <c r="AB80">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AC80">
         <v>0</v>
@@ -43542,7 +43542,7 @@
         <v>0</v>
       </c>
       <c r="AU80">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AV80">
         <v>0</v>
@@ -43596,7 +43596,7 @@
         <v>0</v>
       </c>
       <c r="BM80">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="BN80">
         <v>0</v>
@@ -43896,7 +43896,7 @@
         <v>0</v>
       </c>
       <c r="FI80">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="FJ80">
         <v>0</v>
@@ -44593,7 +44593,7 @@
         <v>0</v>
       </c>
       <c r="AH82">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AI82">
         <v>0</v>
@@ -44728,7 +44728,7 @@
         <v>0</v>
       </c>
       <c r="CA82">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="CB82">
         <v>0</v>
@@ -45001,7 +45001,7 @@
         <v>0</v>
       </c>
       <c r="FN82">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="FO82">
         <v>0</v>
@@ -45222,7 +45222,7 @@
         <v>0</v>
       </c>
       <c r="BJ83">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="BK83">
         <v>0</v>
@@ -45650,7 +45650,7 @@
         <v>0</v>
       </c>
       <c r="W84">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="X84">
         <v>0</v>
@@ -45698,7 +45698,7 @@
         <v>0</v>
       </c>
       <c r="AM84">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AN84">
         <v>0</v>
@@ -45710,7 +45710,7 @@
         <v>0</v>
       </c>
       <c r="AQ84">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AR84">
         <v>0</v>
@@ -46213,7 +46213,7 @@
         <v>0</v>
       </c>
       <c r="AC85">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AD85">
         <v>0</v>
@@ -46303,7 +46303,7 @@
         <v>0</v>
       </c>
       <c r="BG85">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="BH85">
         <v>0</v>
@@ -46758,7 +46758,7 @@
         <v>0</v>
       </c>
       <c r="AC86">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AD86">
         <v>0</v>
@@ -46767,7 +46767,7 @@
         <v>0</v>
       </c>
       <c r="AF86">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AG86">
         <v>0</v>
@@ -46818,7 +46818,7 @@
         <v>0</v>
       </c>
       <c r="AW86">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AX86">
         <v>0</v>
@@ -46902,7 +46902,7 @@
         <v>0</v>
       </c>
       <c r="BY86">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="BZ86">
         <v>0</v>
@@ -47184,7 +47184,7 @@
         <v>0</v>
       </c>
       <c r="FO86">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="FP86">
         <v>0</v>
@@ -47285,7 +47285,7 @@
         <v>0</v>
       </c>
       <c r="W87">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="X87">
         <v>0</v>
@@ -47309,7 +47309,7 @@
         <v>0</v>
       </c>
       <c r="AE87">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AF87">
         <v>0</v>
@@ -47327,7 +47327,7 @@
         <v>0</v>
       </c>
       <c r="AK87">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AL87">
         <v>0</v>
@@ -47339,7 +47339,7 @@
         <v>0</v>
       </c>
       <c r="AO87">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AP87">
         <v>0</v>
@@ -47348,7 +47348,7 @@
         <v>0</v>
       </c>
       <c r="AR87">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AS87">
         <v>0</v>
@@ -47414,7 +47414,7 @@
         <v>0</v>
       </c>
       <c r="BN87">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="BO87">
         <v>0</v>
@@ -47483,7 +47483,7 @@
         <v>0</v>
       </c>
       <c r="CK87">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="CL87">
         <v>0</v>
@@ -47998,7 +47998,7 @@
         <v>0</v>
       </c>
       <c r="CA88">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="CB88">
         <v>0</v>
@@ -48390,7 +48390,7 @@
         <v>0</v>
       </c>
       <c r="AB89">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AC89">
         <v>0</v>
@@ -48408,7 +48408,7 @@
         <v>0</v>
       </c>
       <c r="AH89">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AI89">
         <v>0</v>
@@ -48435,7 +48435,7 @@
         <v>0</v>
       </c>
       <c r="AQ89">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AR89">
         <v>0</v>
@@ -48450,7 +48450,7 @@
         <v>0</v>
       </c>
       <c r="AV89">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AW89">
         <v>0</v>
@@ -48929,7 +48929,7 @@
         <v>0</v>
       </c>
       <c r="Z90">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AA90">
         <v>0</v>
@@ -48974,7 +48974,7 @@
         <v>0</v>
       </c>
       <c r="AO90">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AP90">
         <v>0</v>
@@ -48983,7 +48983,7 @@
         <v>0</v>
       </c>
       <c r="AR90">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AS90">
         <v>0</v>
@@ -49178,10 +49178,10 @@
         <v>0</v>
       </c>
       <c r="DE90">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="DF90">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="DG90">
         <v>0</v>
@@ -49292,7 +49292,7 @@
         <v>0</v>
       </c>
       <c r="EQ90">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="ER90">
         <v>0</v>
@@ -49474,7 +49474,7 @@
         <v>0</v>
       </c>
       <c r="Z91">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AA91">
         <v>0</v>
@@ -49654,7 +49654,7 @@
         <v>0</v>
       </c>
       <c r="CH91">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="CI91">
         <v>0</v>
@@ -49663,7 +49663,7 @@
         <v>0</v>
       </c>
       <c r="CK91">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="CL91">
         <v>0</v>
@@ -51639,7 +51639,7 @@
         <v>0</v>
       </c>
       <c r="U95">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="V95">
         <v>0</v>
@@ -51660,7 +51660,7 @@
         <v>0</v>
       </c>
       <c r="AB95">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AC95">
         <v>0</v>
@@ -51681,7 +51681,7 @@
         <v>0</v>
       </c>
       <c r="AI95">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AJ95">
         <v>0</v>
@@ -51696,10 +51696,10 @@
         <v>0</v>
       </c>
       <c r="AN95">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AO95">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AP95">
         <v>1</v>
@@ -51717,7 +51717,7 @@
         <v>0</v>
       </c>
       <c r="AU95">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AV95">
         <v>0</v>
@@ -51774,7 +51774,7 @@
         <v>0</v>
       </c>
       <c r="BN95">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="BO95">
         <v>0</v>
@@ -51813,7 +51813,7 @@
         <v>0</v>
       </c>
       <c r="CA95">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="CB95">
         <v>0</v>
@@ -52184,7 +52184,7 @@
         <v>0</v>
       </c>
       <c r="U96">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="V96">
         <v>0</v>
@@ -52205,7 +52205,7 @@
         <v>0</v>
       </c>
       <c r="AB96">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AC96">
         <v>0</v>
@@ -52244,7 +52244,7 @@
         <v>0</v>
       </c>
       <c r="AO96">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AP96">
         <v>0</v>
@@ -52262,7 +52262,7 @@
         <v>0</v>
       </c>
       <c r="AU96">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AV96">
         <v>0</v>
@@ -52271,7 +52271,7 @@
         <v>0</v>
       </c>
       <c r="AX96">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AY96">
         <v>0</v>
@@ -52358,10 +52358,10 @@
         <v>0</v>
       </c>
       <c r="CA96">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="CB96">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="CC96">
         <v>0</v>
@@ -52562,7 +52562,7 @@
         <v>0</v>
       </c>
       <c r="EQ96">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="ER96">
         <v>0</v>
@@ -54544,7 +54544,7 @@
         <v>0</v>
       </c>
       <c r="CC100">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="CD100">
         <v>0</v>
@@ -54715,7 +54715,7 @@
         <v>0</v>
       </c>
       <c r="EH100">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="EI100">
         <v>0</v>
@@ -54960,7 +54960,7 @@
         <v>0</v>
       </c>
       <c r="AL101">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AM101">
         <v>0</v>
@@ -54987,7 +54987,7 @@
         <v>0</v>
       </c>
       <c r="AU101">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AV101">
         <v>0</v>
@@ -55071,7 +55071,7 @@
         <v>0</v>
       </c>
       <c r="BW101">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="BX101">
         <v>0</v>
@@ -55101,7 +55101,7 @@
         <v>0</v>
       </c>
       <c r="CG101">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="CH101">
         <v>0</v>
@@ -55538,7 +55538,7 @@
         <v>0</v>
       </c>
       <c r="AW102">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AX102">
         <v>0</v>
@@ -55580,7 +55580,7 @@
         <v>0</v>
       </c>
       <c r="BK102">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="BL102">
         <v>0</v>
@@ -55646,7 +55646,7 @@
         <v>0</v>
       </c>
       <c r="CG102">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="CH102">
         <v>0</v>
@@ -56023,7 +56023,7 @@
         <v>0</v>
       </c>
       <c r="AC103">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AD103">
         <v>0</v>
@@ -56038,7 +56038,7 @@
         <v>0</v>
       </c>
       <c r="AH103">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AI103">
         <v>0</v>
@@ -56263,7 +56263,7 @@
         <v>0</v>
       </c>
       <c r="DE103">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="DF103">
         <v>0</v>
@@ -56610,7 +56610,7 @@
         <v>0</v>
       </c>
       <c r="AQ104">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AR104">
         <v>0</v>
@@ -56625,7 +56625,7 @@
         <v>0</v>
       </c>
       <c r="AV104">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AW104">
         <v>0</v>
@@ -57128,7 +57128,7 @@
         <v>0</v>
       </c>
       <c r="AH105">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AI105">
         <v>0</v>
@@ -57215,7 +57215,7 @@
         <v>0</v>
       </c>
       <c r="BK105">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="BL105">
         <v>0</v>
@@ -57536,7 +57536,7 @@
         <v>0</v>
       </c>
       <c r="FN105">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="FO105">
         <v>0</v>
@@ -57652,19 +57652,19 @@
         <v>0</v>
       </c>
       <c r="AA106">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AB106">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AC106">
         <v>0</v>
       </c>
       <c r="AD106">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AE106">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AF106">
         <v>0</v>
@@ -57748,7 +57748,7 @@
         <v>0</v>
       </c>
       <c r="BG106">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="BH106">
         <v>0</v>
@@ -57913,7 +57913,7 @@
         <v>0</v>
       </c>
       <c r="DJ106">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="DK106">
         <v>0</v>
@@ -58353,7 +58353,7 @@
         <v>0</v>
       </c>
       <c r="CA107">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="CB107">
         <v>0</v>
@@ -58739,7 +58739,7 @@
         <v>0</v>
       </c>
       <c r="Z108">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AA108">
         <v>0</v>
@@ -58907,7 +58907,7 @@
         <v>0</v>
       </c>
       <c r="CD108">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="CE108">
         <v>0</v>
@@ -58988,7 +58988,7 @@
         <v>0</v>
       </c>
       <c r="DE108">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="DF108">
         <v>0</v>
@@ -59392,16 +59392,16 @@
         <v>0</v>
       </c>
       <c r="BJ109">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="BK109">
         <v>0</v>
       </c>
       <c r="BL109">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="BM109">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="BN109">
         <v>0</v>
@@ -59464,7 +59464,7 @@
         <v>0</v>
       </c>
       <c r="CH109">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="CI109">
         <v>0</v>
@@ -59857,7 +59857,7 @@
     </row>
     <row r="19" spans="1:1">
       <c r="A19">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:1">
@@ -59957,7 +59957,7 @@
     </row>
     <row r="39" spans="1:1">
       <c r="A39">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:1">

</xml_diff>